<commit_message>
add Navbar & batch create
</commit_message>
<xml_diff>
--- a/backend/authentication/init_data/staff.xlsx
+++ b/backend/authentication/init_data/staff.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheriewang/git/SE-TSS/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheriewang/git/Data/SE-TSS/backend/authentication/init_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,18 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>教工号</t>
     <rPh sb="0" eb="1">
       <t>jiao'gong'h</t>
@@ -152,7 +140,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A1</t>
+    <t>教务A</t>
+    <rPh sb="0" eb="1">
+      <t>jiao'wu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教务B</t>
+    <rPh sb="0" eb="1">
+      <t>jiao'wu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教务C</t>
+    <rPh sb="0" eb="1">
+      <t>jiao'wu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教务D</t>
+    <rPh sb="0" eb="1">
+      <t>jiao'wu</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,7 +515,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -523,13 +535,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -543,13 +555,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -563,13 +575,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -583,13 +595,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>

</xml_diff>